<commit_message>
Add habitat_typenumbers for P01_1
</commit_message>
<xml_diff>
--- a/analysis/metadata/P01_1/P01_1_minimal_metadata.xlsx
+++ b/analysis/metadata/P01_1/P01_1_minimal_metadata.xlsx
@@ -696,6 +696,11 @@
           <t>agriculture</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
       <c r="G5" t="inlineStr">
         <is>
           <t>kjærsgård</t>
@@ -828,6 +833,11 @@
           <t>agriculture</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>6233</t>
+        </is>
+      </c>
       <c r="G7" t="inlineStr">
         <is>
           <t>uggerby skovvej</t>
@@ -1036,6 +1046,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>9911</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr">
         <is>
           <t>tversted plantage</t>
@@ -1244,6 +1259,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>9915</t>
+        </is>
+      </c>
       <c r="G13" t="inlineStr">
         <is>
           <t>raspkær</t>
@@ -1528,6 +1548,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>6233</t>
+        </is>
+      </c>
       <c r="G17" t="inlineStr">
         <is>
           <t>tjenestejorden</t>
@@ -1584,6 +1609,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>9990</t>
+        </is>
+      </c>
       <c r="G18" t="inlineStr">
         <is>
           <t>tovsigvej</t>
@@ -2248,6 +2278,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>9940</t>
+        </is>
+      </c>
       <c r="G27" t="inlineStr">
         <is>
           <t>rold</t>
@@ -2456,6 +2491,11 @@
           <t>agriculture</t>
         </is>
       </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
       <c r="G30" t="inlineStr">
         <is>
           <t>sønderbyvej</t>
@@ -2664,6 +2704,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>9920</t>
+        </is>
+      </c>
       <c r="G33" t="inlineStr">
         <is>
           <t>ejstrup krat</t>
@@ -2720,6 +2765,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>9920</t>
+        </is>
+      </c>
       <c r="G34" t="inlineStr">
         <is>
           <t>nissum</t>
@@ -2776,6 +2826,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>6233</t>
+        </is>
+      </c>
       <c r="G35" t="inlineStr">
         <is>
           <t>klitvej</t>
@@ -2832,6 +2887,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>9940</t>
+        </is>
+      </c>
       <c r="G36" t="inlineStr">
         <is>
           <t>stråsø plantage</t>
@@ -3192,6 +3252,11 @@
           <t>agriculture</t>
         </is>
       </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>6212</t>
+        </is>
+      </c>
       <c r="G41" t="inlineStr">
         <is>
           <t>lønne</t>
@@ -3400,6 +3465,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>9990</t>
+        </is>
+      </c>
       <c r="G44" t="inlineStr">
         <is>
           <t>filsøvej</t>
@@ -4064,6 +4134,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>9911</t>
+        </is>
+      </c>
       <c r="G53" t="inlineStr">
         <is>
           <t>damvej</t>
@@ -4196,6 +4271,11 @@
           <t>agriculture</t>
         </is>
       </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
       <c r="G55" t="inlineStr">
         <is>
           <t>kalø</t>
@@ -4556,6 +4636,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>9990</t>
+        </is>
+      </c>
       <c r="G60" t="inlineStr">
         <is>
           <t>sletterhage</t>
@@ -4612,6 +4697,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>6402</t>
+        </is>
+      </c>
       <c r="G61" t="inlineStr">
         <is>
           <t>strandkær</t>
@@ -5200,6 +5290,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>9915</t>
+        </is>
+      </c>
       <c r="G69" t="inlineStr">
         <is>
           <t>haarup sande</t>
@@ -5560,6 +5655,11 @@
           <t>agriculture</t>
         </is>
       </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>6233</t>
+        </is>
+      </c>
       <c r="G74" t="inlineStr">
         <is>
           <t>brøndsted fælled</t>
@@ -5616,6 +5716,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>7007</t>
+        </is>
+      </c>
       <c r="G75" t="inlineStr">
         <is>
           <t>rands fjord</t>
@@ -5672,6 +5777,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>6402</t>
+        </is>
+      </c>
       <c r="G76" t="inlineStr">
         <is>
           <t>svinholt</t>
@@ -5728,6 +5838,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>9940</t>
+        </is>
+      </c>
       <c r="G77" t="inlineStr">
         <is>
           <t>vesterskov</t>
@@ -5784,6 +5899,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>9911</t>
+        </is>
+      </c>
       <c r="G78" t="inlineStr">
         <is>
           <t>rand skov</t>
@@ -5840,6 +5960,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>9990</t>
+        </is>
+      </c>
       <c r="G79" t="inlineStr">
         <is>
           <t>grund skov</t>
@@ -6352,6 +6477,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>9920</t>
+        </is>
+      </c>
       <c r="G86" t="inlineStr">
         <is>
           <t>ellemose</t>
@@ -6408,6 +6538,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>9911</t>
+        </is>
+      </c>
       <c r="G87" t="inlineStr">
         <is>
           <t>tisvilde hegn</t>
@@ -6464,6 +6599,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>9990</t>
+        </is>
+      </c>
       <c r="G88" t="inlineStr">
         <is>
           <t>tibberup holme</t>
@@ -7052,6 +7192,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>6233</t>
+        </is>
+      </c>
       <c r="G96" t="inlineStr">
         <is>
           <t>røsnæs</t>
@@ -7260,6 +7405,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>9940</t>
+        </is>
+      </c>
       <c r="G99" t="inlineStr">
         <is>
           <t>broby vesterskov</t>
@@ -7392,6 +7542,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>9920</t>
+        </is>
+      </c>
       <c r="G101" t="inlineStr">
         <is>
           <t>smuldmosen</t>
@@ -7524,6 +7679,11 @@
           <t>agriculture</t>
         </is>
       </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>6233</t>
+        </is>
+      </c>
       <c r="G103" t="inlineStr">
         <is>
           <t>kongskilde friluftsgård</t>
@@ -7580,6 +7740,11 @@
           <t>agriculture</t>
         </is>
       </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
       <c r="G104" t="inlineStr">
         <is>
           <t>fuglebjerg</t>
@@ -7712,6 +7877,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>9990</t>
+        </is>
+      </c>
       <c r="G106" t="inlineStr">
         <is>
           <t>svanninge bakker</t>
@@ -7844,6 +8014,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>9990</t>
+        </is>
+      </c>
       <c r="G108" t="inlineStr">
         <is>
           <t>dalkildegård</t>
@@ -8280,6 +8455,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>9911</t>
+        </is>
+      </c>
       <c r="G114" t="inlineStr">
         <is>
           <t>fuglsang storskov</t>
@@ -8412,6 +8592,11 @@
           <t>agriculture</t>
         </is>
       </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
       <c r="G116" t="inlineStr">
         <is>
           <t>bursø</t>
@@ -8620,6 +8805,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>9920</t>
+        </is>
+      </c>
       <c r="G119" t="inlineStr">
         <is>
           <t>søholt</t>
@@ -8676,6 +8866,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>6402</t>
+        </is>
+      </c>
       <c r="G120" t="inlineStr">
         <is>
           <t>musse mose</t>
@@ -8732,6 +8927,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>6233</t>
+        </is>
+      </c>
       <c r="G121" t="inlineStr">
         <is>
           <t>hejrede sø</t>
@@ -9016,6 +9216,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>6402</t>
+        </is>
+      </c>
       <c r="G125" t="inlineStr">
         <is>
           <t>busemarke mose</t>
@@ -9072,6 +9277,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>6402</t>
+        </is>
+      </c>
       <c r="G126" t="inlineStr">
         <is>
           <t>busemarke sø</t>
@@ -9356,6 +9566,11 @@
           <t>agriculture</t>
         </is>
       </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>6233</t>
+        </is>
+      </c>
       <c r="G130" t="inlineStr">
         <is>
           <t>hegnede bakke</t>
@@ -9414,7 +9629,7 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>9000</t>
+          <t>9940</t>
         </is>
       </c>
       <c r="G131" t="inlineStr">

</xml_diff>

<commit_message>
Revision for ncbi submission
</commit_message>
<xml_diff>
--- a/analysis/metadata/P01_1/P01_1_minimal_metadata.xlsx
+++ b/analysis/metadata/P01_1/P01_1_minimal_metadata.xlsx
@@ -15,9 +15,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -55,12 +52,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,9 +356,6 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="13" max="13" width="20.7109375" style="2" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
@@ -503,8 +496,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M2" s="2">
-        <v>41960</v>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>2014-11-17</t>
+        </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -579,8 +574,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M3" s="2">
-        <v>41961</v>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>2014-11-18</t>
+        </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -655,8 +652,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M4" s="2">
-        <v>41960</v>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>2014-11-17</t>
+        </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -731,8 +730,10 @@
           <t>Agriculture</t>
         </is>
       </c>
-      <c r="M5" s="2">
-        <v>41961</v>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>2014-11-18</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -792,8 +793,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M6" s="2">
-        <v>41961</v>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>2014-11-18</t>
+        </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -868,8 +871,10 @@
           <t>Agriculture</t>
         </is>
       </c>
-      <c r="M7" s="2">
-        <v>41961</v>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>2014-11-18</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -929,8 +934,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M8" s="2">
-        <v>41961</v>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>2014-11-18</t>
+        </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -1005,8 +1012,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M9" s="2">
-        <v>41960</v>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>2014-11-17</t>
+        </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1081,8 +1090,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M10" s="2">
-        <v>41961</v>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>2014-11-18</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -1142,8 +1153,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M11" s="2">
-        <v>41959</v>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>2014-11-16</t>
+        </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1218,8 +1231,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M12" s="2">
-        <v>41959</v>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>2014-11-16</t>
+        </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1294,8 +1309,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M13" s="2">
-        <v>41959</v>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>2014-11-16</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -1355,8 +1372,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M14" s="2">
-        <v>41960</v>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>2014-11-17</t>
+        </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
@@ -1431,8 +1450,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M15" s="2">
-        <v>41959</v>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>2014-11-16</t>
+        </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
@@ -1507,8 +1528,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M16" s="2">
-        <v>41959</v>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>2014-11-16</t>
+        </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
@@ -1583,8 +1606,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M17" s="2">
-        <v>41960</v>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>2014-11-17</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -1644,8 +1669,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M18" s="2">
-        <v>41960</v>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>2014-11-17</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -1705,8 +1732,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M19" s="2">
-        <v>41960</v>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>2014-11-17</t>
+        </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
@@ -1781,8 +1810,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M20" s="2">
-        <v>41962</v>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>2014-11-19</t>
+        </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
@@ -1857,8 +1888,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M21" s="2">
-        <v>41962</v>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>2014-11-19</t>
+        </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
@@ -1933,8 +1966,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M22" s="2">
-        <v>41962</v>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>2014-11-19</t>
+        </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
@@ -2009,8 +2044,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M23" s="2">
-        <v>41962</v>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>2014-11-19</t>
+        </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
@@ -2085,8 +2122,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M24" s="2">
-        <v>41962</v>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>2014-11-19</t>
+        </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
@@ -2161,8 +2200,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M25" s="2">
-        <v>41962</v>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>2014-11-19</t>
+        </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
@@ -2237,8 +2278,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M26" s="2">
-        <v>41962</v>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>2014-11-19</t>
+        </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
@@ -2313,8 +2356,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M27" s="2">
-        <v>41962</v>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>2014-11-19</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -2374,8 +2419,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M28" s="2">
-        <v>41955</v>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>2014-11-12</t>
+        </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
@@ -2450,8 +2497,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M29" s="2">
-        <v>41954</v>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>2014-11-11</t>
+        </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
@@ -2526,8 +2575,10 @@
           <t>Agriculture</t>
         </is>
       </c>
-      <c r="M30" s="2">
-        <v>41955</v>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>2014-11-12</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -2587,8 +2638,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M31" s="2">
-        <v>41955</v>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>2014-11-12</t>
+        </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
@@ -2663,8 +2716,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M32" s="2">
-        <v>41954</v>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>2014-11-11</t>
+        </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
@@ -2739,8 +2794,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M33" s="2">
-        <v>41954</v>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>2014-11-11</t>
+        </is>
       </c>
     </row>
     <row r="34">
@@ -2800,8 +2857,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M34" s="2">
-        <v>41955</v>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>2014-11-12</t>
+        </is>
       </c>
     </row>
     <row r="35">
@@ -2861,8 +2920,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M35" s="2">
-        <v>41955</v>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>2014-11-12</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -2922,8 +2983,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M36" s="2">
-        <v>41955</v>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>2014-11-12</t>
+        </is>
       </c>
     </row>
     <row r="37">
@@ -2983,8 +3046,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M37" s="2">
-        <v>41954</v>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>2014-11-11</t>
+        </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
@@ -3059,8 +3124,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M38" s="2">
-        <v>41954</v>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>2014-11-11</t>
+        </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
@@ -3135,8 +3202,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M39" s="2">
-        <v>41953</v>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>2014-11-10</t>
+        </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
@@ -3211,8 +3280,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M40" s="2">
-        <v>41953</v>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>2014-11-10</t>
+        </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
@@ -3287,8 +3358,10 @@
           <t>Agriculture</t>
         </is>
       </c>
-      <c r="M41" s="2">
-        <v>41954</v>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>2014-11-11</t>
+        </is>
       </c>
     </row>
     <row r="42">
@@ -3348,8 +3421,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M42" s="2">
-        <v>41953</v>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>2014-11-10</t>
+        </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
@@ -3424,8 +3499,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M43" s="2">
-        <v>41953</v>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>2014-11-10</t>
+        </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
@@ -3500,8 +3577,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M44" s="2">
-        <v>41953</v>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>2014-11-10</t>
+        </is>
       </c>
     </row>
     <row r="45">
@@ -3561,8 +3640,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M45" s="2">
-        <v>41949</v>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>2014-11-06</t>
+        </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
@@ -3637,8 +3718,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M46" s="2">
-        <v>41949</v>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>2014-11-06</t>
+        </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
@@ -3713,8 +3796,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M47" s="2">
-        <v>41949</v>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>2014-11-06</t>
+        </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
@@ -3789,8 +3874,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M48" s="2">
-        <v>41949</v>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>2014-11-06</t>
+        </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
@@ -3865,8 +3952,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M49" s="2">
-        <v>41949</v>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>2014-11-06</t>
+        </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
@@ -3941,8 +4030,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M50" s="2">
-        <v>41949</v>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>2014-11-06</t>
+        </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
@@ -4017,8 +4108,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M51" s="2">
-        <v>41949</v>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>2014-11-06</t>
+        </is>
       </c>
       <c r="N51" t="inlineStr">
         <is>
@@ -4093,8 +4186,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M52" s="2">
-        <v>41949</v>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>2014-11-06</t>
+        </is>
       </c>
       <c r="N52" t="inlineStr">
         <is>
@@ -4169,8 +4264,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M53" s="2">
-        <v>41949</v>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>2014-11-06</t>
+        </is>
       </c>
     </row>
     <row r="54">
@@ -4230,8 +4327,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M54" s="2">
-        <v>41956</v>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>2014-11-13</t>
+        </is>
       </c>
       <c r="N54" t="inlineStr">
         <is>
@@ -4306,8 +4405,10 @@
           <t>Agriculture</t>
         </is>
       </c>
-      <c r="M55" s="2">
-        <v>41956</v>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>2014-11-13</t>
+        </is>
       </c>
     </row>
     <row r="56">
@@ -4367,8 +4468,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M56" s="2">
-        <v>41956</v>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>2014-11-13</t>
+        </is>
       </c>
       <c r="N56" t="inlineStr">
         <is>
@@ -4443,8 +4546,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M57" s="2">
-        <v>41956</v>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>2014-11-13</t>
+        </is>
       </c>
       <c r="N57" t="inlineStr">
         <is>
@@ -4519,8 +4624,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M58" s="2">
-        <v>41956</v>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>2014-11-13</t>
+        </is>
       </c>
       <c r="N58" t="inlineStr">
         <is>
@@ -4595,8 +4702,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M59" s="2">
-        <v>41956</v>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>2014-11-13</t>
+        </is>
       </c>
       <c r="N59" t="inlineStr">
         <is>
@@ -4671,8 +4780,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M60" s="2">
-        <v>41956</v>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>2014-11-13</t>
+        </is>
       </c>
     </row>
     <row r="61">
@@ -4732,8 +4843,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M61" s="2">
-        <v>41956</v>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>2014-11-13</t>
+        </is>
       </c>
     </row>
     <row r="62">
@@ -4793,8 +4906,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M62" s="2">
-        <v>41956</v>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>2014-11-13</t>
+        </is>
       </c>
       <c r="N62" t="inlineStr">
         <is>
@@ -4869,8 +4984,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M63" s="2">
-        <v>41930</v>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>2014-10-18</t>
+        </is>
       </c>
       <c r="N63" t="inlineStr">
         <is>
@@ -4945,8 +5062,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M64" s="2">
-        <v>41930</v>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>2014-10-18</t>
+        </is>
       </c>
       <c r="N64" t="inlineStr">
         <is>
@@ -5021,8 +5140,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M65" s="2">
-        <v>41928</v>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>2014-10-16</t>
+        </is>
       </c>
       <c r="N65" t="inlineStr">
         <is>
@@ -5097,8 +5218,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M66" s="2">
-        <v>41930</v>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>2014-10-18</t>
+        </is>
       </c>
       <c r="N66" t="inlineStr">
         <is>
@@ -5173,8 +5296,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M67" s="2">
-        <v>41928</v>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>2014-10-16</t>
+        </is>
       </c>
       <c r="N67" t="inlineStr">
         <is>
@@ -5249,8 +5374,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M68" s="2">
-        <v>41930</v>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>2014-10-18</t>
+        </is>
       </c>
       <c r="N68" t="inlineStr">
         <is>
@@ -5325,8 +5452,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M69" s="2">
-        <v>41930</v>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>2014-10-18</t>
+        </is>
       </c>
     </row>
     <row r="70">
@@ -5386,8 +5515,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M70" s="2">
-        <v>41930</v>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>2014-10-18</t>
+        </is>
       </c>
       <c r="N70" t="inlineStr">
         <is>
@@ -5462,8 +5593,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M71" s="2">
-        <v>41930</v>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>2014-10-18</t>
+        </is>
       </c>
       <c r="N71" t="inlineStr">
         <is>
@@ -5538,8 +5671,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M72" s="2">
-        <v>41947</v>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>2014-11-04</t>
+        </is>
       </c>
       <c r="N72" t="inlineStr">
         <is>
@@ -5614,8 +5749,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M73" s="2">
-        <v>41947</v>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>2014-11-04</t>
+        </is>
       </c>
       <c r="N73" t="inlineStr">
         <is>
@@ -5690,8 +5827,10 @@
           <t>Agriculture</t>
         </is>
       </c>
-      <c r="M74" s="2">
-        <v>41947</v>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>2014-11-04</t>
+        </is>
       </c>
     </row>
     <row r="75">
@@ -5751,8 +5890,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M75" s="2">
-        <v>41947</v>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>2014-11-04</t>
+        </is>
       </c>
     </row>
     <row r="76">
@@ -5812,8 +5953,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M76" s="2">
-        <v>41947</v>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>2014-11-04</t>
+        </is>
       </c>
     </row>
     <row r="77">
@@ -5873,8 +6016,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M77" s="2">
-        <v>41947</v>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>2014-11-04</t>
+        </is>
       </c>
     </row>
     <row r="78">
@@ -5934,8 +6079,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M78" s="2">
-        <v>41947</v>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>2014-11-04</t>
+        </is>
       </c>
     </row>
     <row r="79">
@@ -5995,8 +6142,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M79" s="2">
-        <v>41947</v>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>2014-11-04</t>
+        </is>
       </c>
     </row>
     <row r="80">
@@ -6056,8 +6205,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M80" s="2">
-        <v>41939</v>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>2014-10-27</t>
+        </is>
       </c>
       <c r="N80" t="inlineStr">
         <is>
@@ -6132,8 +6283,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M81" s="2">
-        <v>41939</v>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>2014-10-27</t>
+        </is>
       </c>
       <c r="N81" t="inlineStr">
         <is>
@@ -6208,8 +6361,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M82" s="2">
-        <v>41939</v>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>2014-10-27</t>
+        </is>
       </c>
       <c r="N82" t="inlineStr">
         <is>
@@ -6284,8 +6439,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M83" s="2">
-        <v>41939</v>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>2014-10-27</t>
+        </is>
       </c>
       <c r="N83" t="inlineStr">
         <is>
@@ -6360,8 +6517,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M84" s="2">
-        <v>41939</v>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>2014-10-27</t>
+        </is>
       </c>
       <c r="N84" t="inlineStr">
         <is>
@@ -6436,8 +6595,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M85" s="2">
-        <v>41939</v>
+      <c r="M85" t="inlineStr">
+        <is>
+          <t>2014-10-27</t>
+        </is>
       </c>
       <c r="N85" t="inlineStr">
         <is>
@@ -6512,8 +6673,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M86" s="2">
-        <v>41939</v>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>2014-10-27</t>
+        </is>
       </c>
     </row>
     <row r="87">
@@ -6573,8 +6736,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M87" s="2">
-        <v>41939</v>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>2014-10-27</t>
+        </is>
       </c>
     </row>
     <row r="88">
@@ -6634,8 +6799,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M88" s="2">
-        <v>41939</v>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>2014-10-27</t>
+        </is>
       </c>
     </row>
     <row r="89">
@@ -6695,8 +6862,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M89" s="2">
-        <v>41935</v>
+      <c r="M89" t="inlineStr">
+        <is>
+          <t>2014-10-23</t>
+        </is>
       </c>
       <c r="N89" t="inlineStr">
         <is>
@@ -6771,8 +6940,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M90" s="2">
-        <v>41935</v>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>2014-10-23</t>
+        </is>
       </c>
       <c r="N90" t="inlineStr">
         <is>
@@ -6847,8 +7018,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M91" s="2">
-        <v>41935</v>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>2014-10-23</t>
+        </is>
       </c>
       <c r="N91" t="inlineStr">
         <is>
@@ -6923,8 +7096,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M92" s="2">
-        <v>41935</v>
+      <c r="M92" t="inlineStr">
+        <is>
+          <t>2014-10-23</t>
+        </is>
       </c>
       <c r="N92" t="inlineStr">
         <is>
@@ -6999,8 +7174,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M93" s="2">
-        <v>41935</v>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>2014-10-23</t>
+        </is>
       </c>
       <c r="N93" t="inlineStr">
         <is>
@@ -7075,8 +7252,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M94" s="2">
-        <v>41935</v>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>2014-10-23</t>
+        </is>
       </c>
       <c r="N94" t="inlineStr">
         <is>
@@ -7151,8 +7330,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M95" s="2">
-        <v>41935</v>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>2014-10-23</t>
+        </is>
       </c>
       <c r="N95" t="inlineStr">
         <is>
@@ -7227,8 +7408,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M96" s="2">
-        <v>41935</v>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>2014-10-23</t>
+        </is>
       </c>
     </row>
     <row r="97">
@@ -7288,8 +7471,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M97" s="2">
-        <v>41936</v>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>2014-10-24</t>
+        </is>
       </c>
       <c r="N97" t="inlineStr">
         <is>
@@ -7364,8 +7549,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M98" s="2">
-        <v>41933</v>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>2014-10-21</t>
+        </is>
       </c>
       <c r="N98" t="inlineStr">
         <is>
@@ -7440,8 +7627,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M99" s="2">
-        <v>41933</v>
+      <c r="M99" t="inlineStr">
+        <is>
+          <t>2014-10-21</t>
+        </is>
       </c>
     </row>
     <row r="100">
@@ -7501,8 +7690,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M100" s="2">
-        <v>41936</v>
+      <c r="M100" t="inlineStr">
+        <is>
+          <t>2014-10-24</t>
+        </is>
       </c>
       <c r="N100" t="inlineStr">
         <is>
@@ -7577,8 +7768,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M101" s="2">
-        <v>41936</v>
+      <c r="M101" t="inlineStr">
+        <is>
+          <t>2014-10-24</t>
+        </is>
       </c>
     </row>
     <row r="102">
@@ -7638,8 +7831,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M102" s="2">
-        <v>41933</v>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>2014-10-21</t>
+        </is>
       </c>
       <c r="N102" t="inlineStr">
         <is>
@@ -7714,8 +7909,10 @@
           <t>Agriculture</t>
         </is>
       </c>
-      <c r="M103" s="2">
-        <v>41933</v>
+      <c r="M103" t="inlineStr">
+        <is>
+          <t>2014-10-21</t>
+        </is>
       </c>
     </row>
     <row r="104">
@@ -7775,8 +7972,10 @@
           <t>Agriculture</t>
         </is>
       </c>
-      <c r="M104" s="2">
-        <v>41933</v>
+      <c r="M104" t="inlineStr">
+        <is>
+          <t>2014-10-21</t>
+        </is>
       </c>
     </row>
     <row r="105">
@@ -7836,8 +8035,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M105" s="2">
-        <v>41933</v>
+      <c r="M105" t="inlineStr">
+        <is>
+          <t>2014-10-21</t>
+        </is>
       </c>
       <c r="N105" t="inlineStr">
         <is>
@@ -7912,8 +8113,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M106" s="2">
-        <v>41942</v>
+      <c r="M106" t="inlineStr">
+        <is>
+          <t>2014-10-30</t>
+        </is>
       </c>
     </row>
     <row r="107">
@@ -7973,8 +8176,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M107" s="2">
-        <v>41942</v>
+      <c r="M107" t="inlineStr">
+        <is>
+          <t>2014-10-30</t>
+        </is>
       </c>
       <c r="N107" t="inlineStr">
         <is>
@@ -8049,8 +8254,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M108" s="2">
-        <v>41942</v>
+      <c r="M108" t="inlineStr">
+        <is>
+          <t>2014-10-30</t>
+        </is>
       </c>
     </row>
     <row r="109">
@@ -8110,8 +8317,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M109" s="2">
-        <v>41942</v>
+      <c r="M109" t="inlineStr">
+        <is>
+          <t>2014-10-30</t>
+        </is>
       </c>
       <c r="N109" t="inlineStr">
         <is>
@@ -8186,8 +8395,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M110" s="2">
-        <v>41942</v>
+      <c r="M110" t="inlineStr">
+        <is>
+          <t>2014-10-30</t>
+        </is>
       </c>
       <c r="N110" t="inlineStr">
         <is>
@@ -8262,8 +8473,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M111" s="2">
-        <v>41942</v>
+      <c r="M111" t="inlineStr">
+        <is>
+          <t>2014-10-30</t>
+        </is>
       </c>
       <c r="N111" t="inlineStr">
         <is>
@@ -8338,8 +8551,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M112" s="2">
-        <v>41942</v>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>2014-10-30</t>
+        </is>
       </c>
       <c r="N112" t="inlineStr">
         <is>
@@ -8414,8 +8629,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M113" s="2">
-        <v>41942</v>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>2014-10-30</t>
+        </is>
       </c>
       <c r="N113" t="inlineStr">
         <is>
@@ -8490,8 +8707,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M114" s="2">
-        <v>41940</v>
+      <c r="M114" t="inlineStr">
+        <is>
+          <t>2014-10-28</t>
+        </is>
       </c>
     </row>
     <row r="115">
@@ -8551,8 +8770,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M115" s="2">
-        <v>41940</v>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>2014-10-28</t>
+        </is>
       </c>
       <c r="N115" t="inlineStr">
         <is>
@@ -8627,8 +8848,10 @@
           <t>Agriculture</t>
         </is>
       </c>
-      <c r="M116" s="2">
-        <v>41940</v>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>2014-10-28</t>
+        </is>
       </c>
     </row>
     <row r="117">
@@ -8688,8 +8911,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M117" s="2">
-        <v>41940</v>
+      <c r="M117" t="inlineStr">
+        <is>
+          <t>2014-10-28</t>
+        </is>
       </c>
       <c r="N117" t="inlineStr">
         <is>
@@ -8764,8 +8989,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M118" s="2">
-        <v>41940</v>
+      <c r="M118" t="inlineStr">
+        <is>
+          <t>2014-10-28</t>
+        </is>
       </c>
       <c r="N118" t="inlineStr">
         <is>
@@ -8840,8 +9067,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M119" s="2">
-        <v>41940</v>
+      <c r="M119" t="inlineStr">
+        <is>
+          <t>2014-10-28</t>
+        </is>
       </c>
     </row>
     <row r="120">
@@ -8901,8 +9130,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M120" s="2">
-        <v>41940</v>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>2014-10-28</t>
+        </is>
       </c>
     </row>
     <row r="121">
@@ -8962,8 +9193,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M121" s="2">
-        <v>41940</v>
+      <c r="M121" t="inlineStr">
+        <is>
+          <t>2014-10-28</t>
+        </is>
       </c>
     </row>
     <row r="122">
@@ -9023,8 +9256,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M122" s="2">
-        <v>41932</v>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>2014-10-20</t>
+        </is>
       </c>
       <c r="N122" t="inlineStr">
         <is>
@@ -9099,8 +9334,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M123" s="2">
-        <v>41932</v>
+      <c r="M123" t="inlineStr">
+        <is>
+          <t>2014-10-20</t>
+        </is>
       </c>
       <c r="N123" t="inlineStr">
         <is>
@@ -9175,8 +9412,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M124" s="2">
-        <v>41932</v>
+      <c r="M124" t="inlineStr">
+        <is>
+          <t>2014-10-20</t>
+        </is>
       </c>
       <c r="N124" t="inlineStr">
         <is>
@@ -9251,8 +9490,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M125" s="2">
-        <v>41932</v>
+      <c r="M125" t="inlineStr">
+        <is>
+          <t>2014-10-20</t>
+        </is>
       </c>
     </row>
     <row r="126">
@@ -9312,8 +9553,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M126" s="2">
-        <v>41932</v>
+      <c r="M126" t="inlineStr">
+        <is>
+          <t>2014-10-20</t>
+        </is>
       </c>
     </row>
     <row r="127">
@@ -9373,8 +9616,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M127" s="2">
-        <v>41932</v>
+      <c r="M127" t="inlineStr">
+        <is>
+          <t>2014-10-20</t>
+        </is>
       </c>
       <c r="N127" t="inlineStr">
         <is>
@@ -9449,8 +9694,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M128" s="2">
-        <v>41932</v>
+      <c r="M128" t="inlineStr">
+        <is>
+          <t>2014-10-20</t>
+        </is>
       </c>
       <c r="N128" t="inlineStr">
         <is>
@@ -9525,8 +9772,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M129" s="2">
-        <v>41932</v>
+      <c r="M129" t="inlineStr">
+        <is>
+          <t>2014-10-20</t>
+        </is>
       </c>
       <c r="N129" t="inlineStr">
         <is>
@@ -9601,8 +9850,10 @@
           <t>Agriculture</t>
         </is>
       </c>
-      <c r="M130" s="2">
-        <v>41932</v>
+      <c r="M130" t="inlineStr">
+        <is>
+          <t>2014-10-20</t>
+        </is>
       </c>
     </row>
     <row r="131">
@@ -9662,8 +9913,10 @@
           <t>Natural</t>
         </is>
       </c>
-      <c r="M131" s="2">
-        <v>41932</v>
+      <c r="M131" t="inlineStr">
+        <is>
+          <t>2014-10-20</t>
+        </is>
       </c>
       <c r="N131" t="inlineStr">
         <is>

</xml_diff>